<commit_message>
JTAI refresh, 2025-11-10 14:37:34
</commit_message>
<xml_diff>
--- a/ofsted_csc_jtai_overview.xlsx
+++ b/ofsted_csc_jtai_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="527">
   <si>
     <t>80426</t>
   </si>
@@ -28,7 +28,7 @@
     <t>E08000016</t>
   </si>
   <si>
-    <t>371, 840, 812, 807, 372, 342, 394, 357, 384, 359</t>
+    <t>372, 384, 357, 371, 332, 894, 840, 390, 807, 394</t>
   </si>
   <si>
     <t>barnsley</t>
@@ -67,7 +67,7 @@
     <t>E06000055</t>
   </si>
   <si>
-    <t>831, 881, 919, 886, 887, 826, 940, 941, 866, 937</t>
+    <t>303, 826, 941, 311, 937, 839, 886, 935, 881, 866</t>
   </si>
   <si>
     <t>bedford</t>
@@ -103,7 +103,7 @@
     <t>E06000008</t>
   </si>
   <si>
-    <t>350, 380, 331, 831, 382, 353, 874, 354, 894, 335</t>
+    <t>380, 353, 350, 831, 354, 335, 373, 861, 330, 382</t>
   </si>
   <si>
     <t>blackburn with darwen</t>
@@ -136,7 +136,7 @@
     <t>E06000009</t>
   </si>
   <si>
-    <t>876, 805, 810, 340, 806, 812, 807, 393, 861, 357</t>
+    <t>805, 806, 394, 341, 393, 807, 354, 880, 355, 861</t>
   </si>
   <si>
     <t>blackpool</t>
@@ -172,7 +172,7 @@
     <t>E06000036</t>
   </si>
   <si>
-    <t>825, 823, 850, 919, 931, 803, 358, 869, 938, 816</t>
+    <t>919, 850, 825, 931, 869, 938, 803, 823, 916, 865</t>
   </si>
   <si>
     <t>bracknell forest</t>
@@ -208,7 +208,7 @@
     <t>E06000023</t>
   </si>
   <si>
-    <t>846, 331, 831, 383, 874, 879, 851, 870, 373, 852</t>
+    <t>846, 383, 882, 373, 826, 851, 870, 302, 839, 382</t>
   </si>
   <si>
     <t>bristol</t>
@@ -244,7 +244,7 @@
     <t>E10000002</t>
   </si>
   <si>
-    <t>867, 873, 823, 850, 919, 931, 936, 358, 869, 868</t>
+    <t>931, 919, 869, 936, 873, 867, 823, 868, 358, 850</t>
   </si>
   <si>
     <t>buckinghamshire</t>
@@ -277,7 +277,7 @@
     <t>E06000056</t>
   </si>
   <si>
-    <t>867, 895, 881, 850, 919, 855, 803, 937, 869, 938</t>
+    <t>825, 803, 873, 850, 865, 931, 938, 867, 869, 919</t>
   </si>
   <si>
     <t>central bedfordshire</t>
@@ -310,7 +310,7 @@
     <t>E06000049</t>
   </si>
   <si>
-    <t>823, 896, 811, 850, 855, 802, 815, 877, 937, 885</t>
+    <t>916, 937, 815, 877, 865, 850, 896, 931, 885, 855</t>
   </si>
   <si>
     <t>cheshire east</t>
@@ -343,7 +343,7 @@
     <t>E06000050</t>
   </si>
   <si>
-    <t>895, 811, 881, 891, 334, 860, 356, 877, 937, 885</t>
+    <t>334, 356, 895, 937, 885, 916, 877, 878, 938, 929</t>
   </si>
   <si>
     <t>cheshire west and chester</t>
@@ -376,7 +376,7 @@
     <t>E08000032</t>
   </si>
   <si>
-    <t>889, 350, 831, 332, 382, 353, 874, 354, 894, 335</t>
+    <t>889, 330, 353, 373, 831, 354, 350, 335, 333, 382</t>
   </si>
   <si>
     <t>bradford</t>
@@ -409,7 +409,7 @@
     <t>E06000014</t>
   </si>
   <si>
-    <t>867, 823, 895, 896, 850, 919, 356, 877, 937, 885</t>
+    <t>916, 800, 802, 919, 937, 931, 938, 358, 850, 356</t>
   </si>
   <si>
     <t>york</t>
@@ -439,7 +439,7 @@
     <t>E06000052</t>
   </si>
   <si>
-    <t>878, 838, 845, 884, 921, 925, 926, 893, 933, 935</t>
+    <t>926, 351, 845, 830, 929, 935, 878, 891, 888, 886</t>
   </si>
   <si>
     <t>cornwall</t>
@@ -475,7 +475,7 @@
     <t>E08000026</t>
   </si>
   <si>
-    <t>350, 831, 383, 887, 874, 851, 373, 852, 357, 335</t>
+    <t>831, 852, 874, 350, 336, 312, 354, 335, 821, 861</t>
   </si>
   <si>
     <t>coventry</t>
@@ -511,7 +511,7 @@
     <t>E06000015</t>
   </si>
   <si>
-    <t>350, 331, 332, 382, 383, 887, 874, 373, 894, 335</t>
+    <t>331, 350, 335, 852, 382, 874, 354, 373, 357, 861</t>
   </si>
   <si>
     <t>derby</t>
@@ -544,7 +544,7 @@
     <t>E06000047</t>
   </si>
   <si>
-    <t>370, 841, 390, 392, 807, 342, 808, 394, 384, 359</t>
+    <t>876, 344, 390, 807, 372, 370, 394, 393, 808, 841</t>
   </si>
   <si>
     <t>durham</t>
@@ -577,7 +577,7 @@
     <t>E10000011</t>
   </si>
   <si>
-    <t>839, 878, 838, 881, 886, 926, 802, 933, 935, 885</t>
+    <t>878, 886, 908, 926, 881, 351, 838, 938, 929, 839</t>
   </si>
   <si>
     <t>east sussex</t>
@@ -610,7 +610,7 @@
     <t>E10000013</t>
   </si>
   <si>
-    <t>800, 873, 878, 838, 850, 893, 803, 938, 865, 885</t>
+    <t>937, 938, 850, 802, 865, 895, 855, 931, 881, 885</t>
   </si>
   <si>
     <t>gloucestershire</t>
@@ -643,7 +643,7 @@
     <t>E06000006</t>
   </si>
   <si>
-    <t>370, 841, 840, 805, 340, 806, 812, 807, 393, 394</t>
+    <t>342, 840, 344, 394, 807, 370, 390, 372, 808, 343</t>
   </si>
   <si>
     <t>halton</t>
@@ -676,7 +676,7 @@
     <t>E10000014</t>
   </si>
   <si>
-    <t>873, 823, 916, 919, 855, 802, 803, 937, 938, 885</t>
+    <t>865, 802, 916, 938, 869, 867, 803, 937, 931, 855</t>
   </si>
   <si>
     <t>hampshire</t>
@@ -712,7 +712,7 @@
     <t>E10000015</t>
   </si>
   <si>
-    <t>867, 825, 873, 823, 850, 931, 358, 869, 938, 868</t>
+    <t>931, 825, 873, 867, 938, 305, 850, 358, 916, 869</t>
   </si>
   <si>
     <t>hertfordshire</t>
@@ -748,7 +748,7 @@
     <t>E08000034</t>
   </si>
   <si>
-    <t>350, 351, 381, 831, 332, 888, 383, 354, 808, 894</t>
+    <t>373, 357, 851, 831, 879, 354, 351, 384, 908, 390</t>
   </si>
   <si>
     <t>kirklees</t>
@@ -778,7 +778,7 @@
     <t>E10000017</t>
   </si>
   <si>
-    <t>351, 381, 896, 830, 886, 891, 343, 860, 808, 359</t>
+    <t>925, 351, 332, 884, 841, 808, 384, 891, 929, 359</t>
   </si>
   <si>
     <t>lancashire</t>
@@ -811,7 +811,7 @@
     <t>E08000035</t>
   </si>
   <si>
-    <t>350, 351, 381, 841, 831, 382, 392, 373, 808, 344</t>
+    <t>851, 882, 373, 826, 382, 355, 801, 852, 306, 839</t>
   </si>
   <si>
     <t>leeds</t>
@@ -841,7 +841,7 @@
     <t>E10000019</t>
   </si>
   <si>
-    <t>908, 909, 830, 926, 813, 940, 891, 860, 935, 885</t>
+    <t>888, 384, 884, 813, 926, 935, 332, 940, 830, 933</t>
   </si>
   <si>
     <t>lincolnshire</t>
@@ -877,7 +877,7 @@
     <t>E08000012</t>
   </si>
   <si>
-    <t>841, 390, 876, 805, 340, 806, 391, 355, 393, 394</t>
+    <t>890, 805, 806, 355, 393, 340, 394, 391, 807, 354</t>
   </si>
   <si>
     <t>liverpool</t>
@@ -922,7 +922,7 @@
     <t>E09000004</t>
   </si>
   <si>
-    <t>822, 881, 311, 886, 887, 826, 941, 882, 866, 883</t>
+    <t>311, 822, 886, 881, 883, 887, 826, 866, 839, 351</t>
   </si>
   <si>
     <t>bexley</t>
@@ -955,7 +955,7 @@
     <t>E09000006</t>
   </si>
   <si>
-    <t>822, 867, 823, 850, 919, 931, 334, 356, 319, 358</t>
+    <t>919, 358, 825, 869, 867, 931, 850, 868, 334, 936</t>
   </si>
   <si>
     <t>bromley</t>
@@ -988,7 +988,7 @@
     <t>E09000008</t>
   </si>
   <si>
-    <t>330, 304, 307, 308, 203, 309, 208, 209, 315, 320</t>
+    <t>209, 320, 383, 870, 826, 882, 302, 852, 355, 203</t>
   </si>
   <si>
     <t>croydon</t>
@@ -1021,7 +1021,7 @@
     <t>E09000011</t>
   </si>
   <si>
-    <t>301, 307, 308, 205, 309, 352, 315, 870, 210, 320</t>
+    <t>209, 208, 306, 210, 355, 320, 851, 852, 391, 870</t>
   </si>
   <si>
     <t>greenwich</t>
@@ -1054,7 +1054,7 @@
     <t>E09000014</t>
   </si>
   <si>
-    <t>306, 308, 203, 204, 205, 206, 208, 209, 210, 320</t>
+    <t>320, 307, 209, 208, 302, 308, 210, 304, 313, 317</t>
   </si>
   <si>
     <t>haringey</t>
@@ -1087,7 +1087,7 @@
     <t>E09000015</t>
   </si>
   <si>
-    <t>302, 304, 307, 312, 313, 314, 315, 317, 871, 319</t>
+    <t>317, 312, 302, 307, 320, 870, 313, 315, 871, 826</t>
   </si>
   <si>
     <t>harrow</t>
@@ -1111,6 +1111,39 @@
     <t>The strategic oversight and scrutiny from the HSSP of the MASH and the provision of early support. The location of the MASH to ensure that agencies are co-located safely and are supported to assess risk and make timely joint decisions. The capacity of police and health resources to support the work in the MASH.</t>
   </si>
   <si>
+    <t>80501</t>
+  </si>
+  <si>
+    <t>312</t>
+  </si>
+  <si>
+    <t>E09000017</t>
+  </si>
+  <si>
+    <t>313, 317, 320, 874, 307, 852, 310, 870, 871, 331</t>
+  </si>
+  <si>
+    <t>hillingdon</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50284538</t>
+  </si>
+  <si>
+    <t>14/08/25</t>
+  </si>
+  <si>
+    <t>Children who are victims of domestic abuse in hillingdon.</t>
+  </si>
+  <si>
+    <t>The members of the partnership know themselves well and understand that they need to strengthen the response to victims of domestic abuse in Hillingdon. The partnership leaders response to the inspection findings and their commitment to implement changes to better support victims of domestic abuse. The partnership has recently put in place well-considered and robust governance arrangements aimed at providing a framework to support a more effective approach to tackling domestic abuse.</t>
+  </si>
+  <si>
+    <t>Leaders across agencies have recognised that their collective strategic cooperation, governance and oversight of domestic abuse has not been effective enough. The absence of a strategic needs analysis of domestic abuse and the support to victims was insufficient. In response, since June 2024, partner agencies, working together through the Safer Hillingdon Partnership (SHP), are formulating a clearer delivery plan, to prioritise tackling domestic abuse.</t>
+  </si>
+  <si>
+    <t>How effectively the multi-agency public protection arrangements (MAPPA) and multi-agency risk assessment conference (MARAC) processes are being used to protect children and adults from domestic abuse and how well these processes are integrated with, and used to inform, wider work to support and protect children and families. Strategic and operational links between probation and the partnership, in particular with regard to strengthening the effectiveness of disruption activity. The effectiveness of multi-agency joint working, in strategic and operational contexts, to tackle domestic abuse.</t>
+  </si>
+  <si>
     <t>80503</t>
   </si>
   <si>
@@ -1120,7 +1153,7 @@
     <t>E09000018</t>
   </si>
   <si>
-    <t>302, 307, 310, 312, 856, 315, 870, 317, 871, 319</t>
+    <t>307, 312, 871, 317, 320, 821, 304, 310, 852, 301</t>
   </si>
   <si>
     <t>hounslow</t>
@@ -1153,7 +1186,7 @@
     <t>E09000019</t>
   </si>
   <si>
-    <t>202, 203, 204, 205, 309, 208, 352, 210, 212, 213</t>
+    <t>202, 210, 208, 213, 204, 205, 209, 309, 203, 352</t>
   </si>
   <si>
     <t>islington</t>
@@ -1183,7 +1216,7 @@
     <t>E09000023</t>
   </si>
   <si>
-    <t>304, 306, 308, 203, 204, 205, 309, 208, 210, 320</t>
+    <t>208, 210, 306, 205, 203, 320, 309, 302, 383, 355</t>
   </si>
   <si>
     <t>lewisham</t>
@@ -1216,7 +1249,7 @@
     <t>E09000024</t>
   </si>
   <si>
-    <t>302, 307, 308, 312, 313, 314, 870, 317, 319, 212</t>
+    <t>319, 314, 870, 302, 826, 822, 306, 919, 310, 873</t>
   </si>
   <si>
     <t>merton</t>
@@ -1249,7 +1282,7 @@
     <t>E09000027</t>
   </si>
   <si>
-    <t>305, 825, 873, 919, 314, 931, 936, 869, 868, 872</t>
+    <t>868, 314, 936, 872, 305, 358, 825, 919, 800, 869</t>
   </si>
   <si>
     <t>richmond upon thames</t>
@@ -1282,7 +1315,7 @@
     <t>E09000029</t>
   </si>
   <si>
-    <t>302, 822, 303, 867, 305, 919, 314, 826, 870, 866</t>
+    <t>315, 919, 826, 873, 931, 314, 822, 938, 839, 825</t>
   </si>
   <si>
     <t>sutton</t>
@@ -1315,7 +1348,7 @@
     <t>E08000003</t>
   </si>
   <si>
-    <t>330, 801, 341, 391, 892, 851, 355, 373, 852, 336</t>
+    <t>892, 330, 391, 308, 380, 355, 806, 852, 309, 353</t>
   </si>
   <si>
     <t>manchester</t>
@@ -1351,7 +1384,7 @@
     <t>E06000035</t>
   </si>
   <si>
-    <t>332, 311, 886, 940, 941, 372, 882, 866, 894, 883</t>
+    <t>866, 332, 886, 303, 926, 935, 883, 891, 351, 384</t>
   </si>
   <si>
     <t>medway</t>
@@ -1387,7 +1420,7 @@
     <t>E06000042</t>
   </si>
   <si>
-    <t>822, 303, 831, 919, 886, 383, 941, 870, 866, 883</t>
+    <t>822, 303, 882, 870, 839, 311, 919, 886, 319, 383</t>
   </si>
   <si>
     <t>milton keynes</t>
@@ -1420,7 +1453,7 @@
     <t>E10000020</t>
   </si>
   <si>
-    <t>908, 909, 878, 838, 845, 921, 925, 893, 933, 935</t>
+    <t>935, 908, 878, 830, 929, 886, 933, 925, 891, 887</t>
   </si>
   <si>
     <t>norfolk</t>
@@ -1444,6 +1477,39 @@
     <t>Partners understanding and engagement in MARAC and the Partnerships oversight of its operation. The consistent consideration of the cumulative harm to children aged 0 to 7 from repeated experience of domestic violence. How well the voices and experiences of individual children who are victims of domestic abuse are listened to, understood and captured by practitioners, across the partnership, and are used to inform childrens plans.</t>
   </si>
   <si>
+    <t>80530</t>
+  </si>
+  <si>
+    <t>815</t>
+  </si>
+  <si>
+    <t>E10000023</t>
+  </si>
+  <si>
+    <t>893, 895, 811, 860, 916, 877, 937, 884, 865, 933</t>
+  </si>
+  <si>
+    <t>north yorkshire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50272930</t>
+  </si>
+  <si>
+    <t>28/03/25</t>
+  </si>
+  <si>
+    <t>Unborn children and those aged 0 to 7 who are victims of domestic abuse in north yorkshire.</t>
+  </si>
+  <si>
+    <t>The mature and respectful relationships between statutory and community partners in the North Yorkshire Safeguarding Children Partnership (NYCSP), the Domestic Abuse Local Partnership Board (DALPB) and the Community Safety Partnership (CSP). The effective use of a practice model in childrens social care and early help as a vehicle for giving families the skills and insight they need to protect their children from domestic abuse. The quality of direct work with children to help them understand what is happening to them and their family.</t>
+  </si>
+  <si>
+    <t>Unborn children, and those aged 0 to 7 who are victims of domestic abuse in North Yorkshire, are seen, understood and safeguarded by professionals and key people in their own communities. North Yorkshire is a large and complex county where children live in coastal, holiday towns with seasonal poverty, on the outskirts of neighbouring cities, in small towns (including an army garrison the size of a small town) and many attend small rural schools. The response to domestic abuse in a place of this scale is consistent in its localism, informed by clear and decisive strategic intent and delivered by skilled practitioners who understand the impact of domestic abuse on young children.</t>
+  </si>
+  <si>
+    <t>How the experiences of child victims of domestic abuse aged 0 to 7 are consistently captured across the partnership. The extent to which children are recognised as victims of domestic abuse in their own right across the partnership. The timeliness and consistency of information-sharing across the partnership to inform risk assessments and safety planning.</t>
+  </si>
+  <si>
     <t>80532</t>
   </si>
   <si>
@@ -1453,7 +1519,7 @@
     <t>E06000057</t>
   </si>
   <si>
-    <t>381, 896, 830, 811, 888, 392, 891, 860, 808, 877</t>
+    <t>926, 830, 888, 908, 878, 840, 838, 886, 885, 935</t>
   </si>
   <si>
     <t>northumberland</t>
@@ -1891,7 +1957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1899,58 +1965,58 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>487</v>
+        <v>509</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>488</v>
+        <v>510</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>489</v>
+        <v>511</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>490</v>
+        <v>512</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>491</v>
+        <v>513</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>492</v>
+        <v>514</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>493</v>
+        <v>515</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>494</v>
+        <v>516</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>495</v>
+        <v>517</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>497</v>
+        <v>519</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>498</v>
+        <v>520</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>499</v>
+        <v>521</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>500</v>
+        <v>522</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>501</v>
+        <v>523</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>502</v>
+        <v>524</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>503</v>
+        <v>525</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>504</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -3806,7 +3872,7 @@
         <v>371</v>
       </c>
       <c r="J34" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80501_hillingdon", ".\export_data\inspection_reports\80501_hillingdon")</f>
         <v>0</v>
       </c>
       <c r="K34" t="s">
@@ -3816,22 +3882,22 @@
         <v>9</v>
       </c>
       <c r="M34" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" t="s">
         <v>373</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>374</v>
       </c>
-      <c r="O34" t="s">
-        <v>9</v>
-      </c>
       <c r="P34" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="Q34" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R34" t="s">
-        <v>375</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -3863,7 +3929,7 @@
         <v>382</v>
       </c>
       <c r="J35" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
         <v>0</v>
       </c>
       <c r="K35" t="s">
@@ -3885,61 +3951,61 @@
         <v>9</v>
       </c>
       <c r="Q35" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="R35" t="s">
-        <v>9</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B36" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C36" t="s">
         <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E36" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F36" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H36" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I36" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="J36" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
         <v>0</v>
       </c>
       <c r="K36" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L36" t="s">
         <v>9</v>
       </c>
       <c r="M36" t="s">
-        <v>9</v>
+        <v>395</v>
       </c>
       <c r="N36" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="O36" t="s">
-        <v>395</v>
+        <v>9</v>
       </c>
       <c r="P36" t="s">
-        <v>396</v>
+        <v>9</v>
       </c>
       <c r="Q36" t="s">
         <v>12</v>
@@ -3977,7 +4043,7 @@
         <v>403</v>
       </c>
       <c r="J37" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
         <v>0</v>
       </c>
       <c r="K37" t="s">
@@ -4034,7 +4100,7 @@
         <v>414</v>
       </c>
       <c r="J38" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
         <v>0</v>
       </c>
       <c r="K38" t="s">
@@ -4091,7 +4157,7 @@
         <v>425</v>
       </c>
       <c r="J39" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
         <v>0</v>
       </c>
       <c r="K39" t="s">
@@ -4127,7 +4193,7 @@
         <v>431</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>300</v>
       </c>
       <c r="D40" t="s">
         <v>432</v>
@@ -4148,7 +4214,7 @@
         <v>436</v>
       </c>
       <c r="J40" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
         <v>0</v>
       </c>
       <c r="K40" t="s">
@@ -4184,107 +4250,107 @@
         <v>442</v>
       </c>
       <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
         <v>443</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>444</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>445</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" t="s">
         <v>447</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
+        <v>447</v>
+      </c>
+      <c r="J41" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
         <v>448</v>
       </c>
-      <c r="I41" t="s">
-        <v>448</v>
-      </c>
-      <c r="J41" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
-        <v>0</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
         <v>449</v>
       </c>
-      <c r="L41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M41" t="s">
+      <c r="O41" t="s">
         <v>450</v>
       </c>
-      <c r="N41" t="s">
+      <c r="P41" t="s">
         <v>451</v>
       </c>
-      <c r="O41" t="s">
-        <v>9</v>
-      </c>
-      <c r="P41" t="s">
-        <v>9</v>
-      </c>
       <c r="Q41" t="s">
-        <v>452</v>
+        <v>12</v>
       </c>
       <c r="R41" t="s">
-        <v>453</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:18">
       <c r="A42" t="s">
+        <v>452</v>
+      </c>
+      <c r="B42" t="s">
+        <v>453</v>
+      </c>
+      <c r="C42" t="s">
         <v>454</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>455</v>
       </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>456</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>457</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" t="s">
         <v>459</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
+        <v>459</v>
+      </c>
+      <c r="J42" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
         <v>460</v>
       </c>
-      <c r="I42" t="s">
-        <v>460</v>
-      </c>
-      <c r="J42" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
         <v>461</v>
       </c>
-      <c r="L42" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>462</v>
       </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
+        <v>9</v>
+      </c>
+      <c r="P42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" t="s">
         <v>463</v>
-      </c>
-      <c r="O42" t="s">
-        <v>9</v>
-      </c>
-      <c r="P42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>71</v>
       </c>
       <c r="R42" t="s">
         <v>464</v>
@@ -4298,7 +4364,7 @@
         <v>466</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s">
         <v>467</v>
@@ -4319,7 +4385,7 @@
         <v>471</v>
       </c>
       <c r="J43" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
         <v>0</v>
       </c>
       <c r="K43" t="s">
@@ -4329,22 +4395,22 @@
         <v>9</v>
       </c>
       <c r="M43" t="s">
-        <v>9</v>
+        <v>473</v>
       </c>
       <c r="N43" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="O43" t="s">
-        <v>474</v>
+        <v>9</v>
       </c>
       <c r="P43" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>71</v>
+      </c>
+      <c r="R43" t="s">
         <v>475</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>12</v>
-      </c>
-      <c r="R43" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -4355,7 +4421,7 @@
         <v>477</v>
       </c>
       <c r="C44" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
         <v>478</v>
@@ -4376,32 +4442,146 @@
         <v>482</v>
       </c>
       <c r="J44" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>483</v>
+      </c>
+      <c r="L44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" t="s">
+        <v>9</v>
+      </c>
+      <c r="N44" t="s">
+        <v>484</v>
+      </c>
+      <c r="O44" t="s">
+        <v>485</v>
+      </c>
+      <c r="P44" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>12</v>
+      </c>
+      <c r="R44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" t="s">
+        <v>487</v>
+      </c>
+      <c r="B45" t="s">
+        <v>488</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>489</v>
+      </c>
+      <c r="E45" t="s">
+        <v>490</v>
+      </c>
+      <c r="F45" t="s">
+        <v>491</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="H45" t="s">
+        <v>493</v>
+      </c>
+      <c r="I45" t="s">
+        <v>493</v>
+      </c>
+      <c r="J45" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
+        <v>494</v>
+      </c>
+      <c r="L45" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" t="s">
+        <v>9</v>
+      </c>
+      <c r="N45" t="s">
+        <v>495</v>
+      </c>
+      <c r="O45" t="s">
+        <v>496</v>
+      </c>
+      <c r="P45" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>12</v>
+      </c>
+      <c r="R45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" t="s">
+        <v>498</v>
+      </c>
+      <c r="B46" t="s">
+        <v>499</v>
+      </c>
+      <c r="C46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" t="s">
+        <v>500</v>
+      </c>
+      <c r="E46" t="s">
+        <v>501</v>
+      </c>
+      <c r="F46" t="s">
+        <v>502</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="H46" t="s">
+        <v>504</v>
+      </c>
+      <c r="I46" t="s">
+        <v>504</v>
+      </c>
+      <c r="J46" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80532_northumberland", ".\export_data\inspection_reports\80532_northumberland")</f>
         <v>0</v>
       </c>
-      <c r="K44" t="s">
-        <v>483</v>
-      </c>
-      <c r="L44" t="s">
-        <v>9</v>
-      </c>
-      <c r="M44" t="s">
-        <v>484</v>
-      </c>
-      <c r="N44" t="s">
-        <v>485</v>
-      </c>
-      <c r="O44" t="s">
-        <v>9</v>
-      </c>
-      <c r="P44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q44" t="s">
+      <c r="K46" t="s">
+        <v>505</v>
+      </c>
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>506</v>
+      </c>
+      <c r="N46" t="s">
+        <v>507</v>
+      </c>
+      <c r="O46" t="s">
+        <v>9</v>
+      </c>
+      <c r="P46" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q46" t="s">
         <v>71</v>
       </c>
-      <c r="R44" t="s">
-        <v>486</v>
+      <c r="R46" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -4449,6 +4629,8 @@
     <hyperlink ref="G42" r:id="rId41"/>
     <hyperlink ref="G43" r:id="rId42"/>
     <hyperlink ref="G44" r:id="rId43"/>
+    <hyperlink ref="G45" r:id="rId44"/>
+    <hyperlink ref="G46" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
JTAI refresh, 2025-12-08 05:07:09
</commit_message>
<xml_diff>
--- a/ofsted_csc_jtai_overview.xlsx
+++ b/ofsted_csc_jtai_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="538">
   <si>
     <t>80426</t>
   </si>
@@ -194,6 +194,39 @@
   </si>
   <si>
     <t>Multi-agency strengths Senior leaders and managers in Bracknell Forest have positive and productive working relationships. There is a shared ambition to ensure that high-quality services are available for children, as well as a determination to continuously improve services, systems and processes. Some partners face challenges in fulfilling their role in Bracknell Forest as a result of their wider responsibilities in the region.</t>
+  </si>
+  <si>
+    <t>80438</t>
+  </si>
+  <si>
+    <t>846</t>
+  </si>
+  <si>
+    <t>E06000043</t>
+  </si>
+  <si>
+    <t>801, 882, 302, 314, 800, 383, 209, 826, 212, 816</t>
+  </si>
+  <si>
+    <t>brighton and hove</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50292133</t>
+  </si>
+  <si>
+    <t>04/12/25</t>
+  </si>
+  <si>
+    <t>Child sexual abuse in the family environment in brighton and hove.</t>
+  </si>
+  <si>
+    <t>. All references to children in this letter relate to children at risk or victims of child sexual abuse in the family environment. We anticipate that these JTAIs will identify learning for all agencies and will contribute to the debate about what good practice looks like.</t>
+  </si>
+  <si>
+    <t>Professionals across the partnership demonstrate high levels of commitment, thoughtfulness and reflection to engage sensitively with families and build trust. Prior to this inspection, the multi-agency safeguarding partnership had already recognised the need to make improvements to the response of services to child sexual abuse in the family environment in Brighton and Hove. It responded quickly to the findings of 2 the CSPRP report last year and had promptly agreed the need for a plan to understand the prevalence and the needs of these children.</t>
+  </si>
+  <si>
+    <t>Joint multi-agency information-sharing and decision-making, particularly in strategy and child in need meetings. The quality and involvement from relevant partners in ongoing multi-agency assessment and planning for children in need and their families in relation to child sexual abuse in the family environment. The timeliness of police investigations to ensure families and the professional network are regularly updated about progress.</t>
   </si>
   <si>
     <t>80441</t>
@@ -1957,7 +1990,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1965,58 +1998,58 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>519</v>
+        <v>530</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>520</v>
+        <v>531</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>526</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -2312,110 +2345,110 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>64</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" t="s">
         <v>66</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80438_brighton and hove", ".\export_data\inspection_reports\80438_brighton and hove")</f>
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>67</v>
       </c>
-      <c r="I7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80441_bristol", ".\export_data\inspection_reports\80441_bristol")</f>
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" t="s">
         <v>68</v>
       </c>
-      <c r="L7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>69</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>70</v>
       </c>
-      <c r="O7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" t="s">
-        <v>9</v>
-      </c>
       <c r="Q7" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R7" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" t="s">
         <v>78</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80441_bristol", ".\export_data\inspection_reports\80441_bristol")</f>
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
         <v>79</v>
       </c>
-      <c r="I8" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80442_buckinghamshire", ".\export_data\inspection_reports\80442_buckinghamshire")</f>
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
         <v>80</v>
-      </c>
-      <c r="L8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" t="s">
-        <v>9</v>
       </c>
       <c r="N8" t="s">
         <v>81</v>
       </c>
       <c r="O8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" t="s">
         <v>82</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>83</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>12</v>
-      </c>
-      <c r="R8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -2426,7 +2459,7 @@
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>86</v>
@@ -2447,7 +2480,7 @@
         <v>90</v>
       </c>
       <c r="J9" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80446_central bedfordshire", ".\export_data\inspection_reports\80446_central bedfordshire")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80442_buckinghamshire", ".\export_data\inspection_reports\80442_buckinghamshire")</f>
         <v>0</v>
       </c>
       <c r="K9" t="s">
@@ -2457,22 +2490,22 @@
         <v>9</v>
       </c>
       <c r="M9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" t="s">
         <v>92</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>93</v>
       </c>
-      <c r="O9" t="s">
-        <v>9</v>
-      </c>
       <c r="P9" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="Q9" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -2483,7 +2516,7 @@
         <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>97</v>
@@ -2504,7 +2537,7 @@
         <v>101</v>
       </c>
       <c r="J10" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80447_cheshire east", ".\export_data\inspection_reports\80447_cheshire east")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80446_central bedfordshire", ".\export_data\inspection_reports\80446_central bedfordshire")</f>
         <v>0</v>
       </c>
       <c r="K10" t="s">
@@ -2514,22 +2547,22 @@
         <v>9</v>
       </c>
       <c r="M10" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="N10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" t="s">
         <v>105</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>12</v>
-      </c>
-      <c r="R10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -2561,7 +2594,7 @@
         <v>112</v>
       </c>
       <c r="J11" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80448_cheshire west and chester", ".\export_data\inspection_reports\80448_cheshire west and chester")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80447_cheshire east", ".\export_data\inspection_reports\80447_cheshire east")</f>
         <v>0</v>
       </c>
       <c r="K11" t="s">
@@ -2571,22 +2604,22 @@
         <v>9</v>
       </c>
       <c r="M11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
         <v>114</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>115</v>
       </c>
-      <c r="O11" t="s">
-        <v>9</v>
-      </c>
       <c r="P11" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="Q11" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R11" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -2597,7 +2630,7 @@
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>119</v>
@@ -2618,7 +2651,7 @@
         <v>123</v>
       </c>
       <c r="J12" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80449_bradford", ".\export_data\inspection_reports\80449_bradford")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80448_cheshire west and chester", ".\export_data\inspection_reports\80448_cheshire west and chester")</f>
         <v>0</v>
       </c>
       <c r="K12" t="s">
@@ -2640,7 +2673,7 @@
         <v>9</v>
       </c>
       <c r="Q12" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R12" t="s">
         <v>127</v>
@@ -2675,7 +2708,7 @@
         <v>134</v>
       </c>
       <c r="J13" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80453_york", ".\export_data\inspection_reports\80453_york")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80449_bradford", ".\export_data\inspection_reports\80449_bradford")</f>
         <v>0</v>
       </c>
       <c r="K13" t="s">
@@ -2697,49 +2730,49 @@
         <v>9</v>
       </c>
       <c r="Q13" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="R13" t="s">
-        <v>9</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J14" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80454_cornwall", ".\export_data\inspection_reports\80454_cornwall")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80453_york", ".\export_data\inspection_reports\80453_york")</f>
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L14" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="M14" t="s">
         <v>147</v>
@@ -2768,47 +2801,47 @@
         <v>150</v>
       </c>
       <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
         <v>151</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>152</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>153</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" t="s">
         <v>155</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80454_cornwall", ".\export_data\inspection_reports\80454_cornwall")</f>
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
         <v>156</v>
       </c>
-      <c r="I15" t="s">
-        <v>156</v>
-      </c>
-      <c r="J15" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80456_coventry", ".\export_data\inspection_reports\80456_coventry")</f>
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>157</v>
       </c>
-      <c r="L15" t="s">
-        <v>9</v>
-      </c>
       <c r="M15" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="N15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="O15" t="s">
-        <v>159</v>
+        <v>9</v>
       </c>
       <c r="P15" t="s">
-        <v>160</v>
+        <v>9</v>
       </c>
       <c r="Q15" t="s">
         <v>12</v>
@@ -2819,53 +2852,53 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
         <v>161</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>162</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>163</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>164</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>165</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" t="s">
         <v>167</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80456_coventry", ".\export_data\inspection_reports\80456_coventry")</f>
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
         <v>168</v>
       </c>
-      <c r="I16" t="s">
-        <v>168</v>
-      </c>
-      <c r="J16" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80459_derby", ".\export_data\inspection_reports\80459_derby")</f>
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
         <v>169</v>
       </c>
-      <c r="L16" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>170</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>171</v>
-      </c>
-      <c r="O16" t="s">
-        <v>9</v>
-      </c>
-      <c r="P16" t="s">
-        <v>9</v>
       </c>
       <c r="Q16" t="s">
         <v>12</v>
@@ -2903,20 +2936,20 @@
         <v>179</v>
       </c>
       <c r="J17" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80465_durham", ".\export_data\inspection_reports\80465_durham")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80459_derby", ".\export_data\inspection_reports\80459_derby")</f>
         <v>0</v>
       </c>
       <c r="K17" t="s">
         <v>180</v>
       </c>
       <c r="L17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" t="s">
         <v>181</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>182</v>
-      </c>
-      <c r="N17" t="s">
-        <v>183</v>
       </c>
       <c r="O17" t="s">
         <v>9</v>
@@ -2933,13 +2966,13 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
         <v>184</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>185</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
       </c>
       <c r="D18" t="s">
         <v>186</v>
@@ -2960,20 +2993,20 @@
         <v>190</v>
       </c>
       <c r="J18" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80467_east sussex", ".\export_data\inspection_reports\80467_east sussex")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80465_durham", ".\export_data\inspection_reports\80465_durham")</f>
         <v>0</v>
       </c>
       <c r="K18" t="s">
         <v>191</v>
       </c>
       <c r="L18" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O18" t="s">
         <v>9</v>
@@ -2982,10 +3015,10 @@
         <v>9</v>
       </c>
       <c r="Q18" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R18" t="s">
-        <v>194</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2996,7 +3029,7 @@
         <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>197</v>
@@ -3017,7 +3050,7 @@
         <v>201</v>
       </c>
       <c r="J19" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80470_gloucestershire", ".\export_data\inspection_reports\80470_gloucestershire")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80467_east sussex", ".\export_data\inspection_reports\80467_east sussex")</f>
         <v>0</v>
       </c>
       <c r="K19" t="s">
@@ -3027,22 +3060,22 @@
         <v>9</v>
       </c>
       <c r="M19" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
       <c r="N19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O19" t="s">
-        <v>204</v>
+        <v>9</v>
       </c>
       <c r="P19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>82</v>
+      </c>
+      <c r="R19" t="s">
         <v>205</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>12</v>
-      </c>
-      <c r="R19" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -3053,7 +3086,7 @@
         <v>207</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
         <v>208</v>
@@ -3074,7 +3107,7 @@
         <v>212</v>
       </c>
       <c r="J20" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80471_halton", ".\export_data\inspection_reports\80471_halton")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80470_gloucestershire", ".\export_data\inspection_reports\80470_gloucestershire")</f>
         <v>0</v>
       </c>
       <c r="K20" t="s">
@@ -3084,22 +3117,22 @@
         <v>9</v>
       </c>
       <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" t="s">
         <v>214</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>215</v>
       </c>
-      <c r="O20" t="s">
-        <v>9</v>
-      </c>
       <c r="P20" t="s">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="Q20" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R20" t="s">
-        <v>216</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -3110,7 +3143,7 @@
         <v>218</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
         <v>219</v>
@@ -3128,67 +3161,67 @@
         <v>223</v>
       </c>
       <c r="I21" t="s">
+        <v>223</v>
+      </c>
+      <c r="J21" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80471_halton", ".\export_data\inspection_reports\80471_halton")</f>
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
         <v>224</v>
       </c>
-      <c r="J21" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80472_hampshire", ".\export_data\inspection_reports\80472_hampshire")</f>
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" t="s">
         <v>225</v>
       </c>
-      <c r="L21" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>226</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>82</v>
+      </c>
+      <c r="R21" t="s">
         <v>227</v>
-      </c>
-      <c r="O21" t="s">
-        <v>9</v>
-      </c>
-      <c r="P21" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>71</v>
-      </c>
-      <c r="R21" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" t="s">
         <v>229</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
         <v>230</v>
       </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>231</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>232</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" t="s">
         <v>234</v>
-      </c>
-      <c r="H22" t="s">
-        <v>235</v>
       </c>
       <c r="I22" t="s">
         <v>235</v>
       </c>
       <c r="J22" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80475_hertfordshire", ".\export_data\inspection_reports\80475_hertfordshire")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80472_hampshire", ".\export_data\inspection_reports\80472_hampshire")</f>
         <v>0</v>
       </c>
       <c r="K22" t="s">
@@ -3204,67 +3237,67 @@
         <v>238</v>
       </c>
       <c r="O22" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>82</v>
+      </c>
+      <c r="R22" t="s">
         <v>239</v>
-      </c>
-      <c r="P22" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>12</v>
-      </c>
-      <c r="R22" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23" t="s">
         <v>241</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
         <v>242</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>243</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>244</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" t="s">
         <v>246</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>246</v>
+      </c>
+      <c r="J23" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80475_hertfordshire", ".\export_data\inspection_reports\80475_hertfordshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
         <v>247</v>
       </c>
-      <c r="I23" t="s">
-        <v>247</v>
-      </c>
-      <c r="J23" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80478_kirklees", ".\export_data\inspection_reports\80478_kirklees")</f>
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
         <v>248</v>
       </c>
-      <c r="L23" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" t="s">
-        <v>9</v>
-      </c>
       <c r="N23" t="s">
-        <v>9</v>
+        <v>249</v>
       </c>
       <c r="O23" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="P23" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Q23" t="s">
         <v>12</v>
@@ -3275,38 +3308,38 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I24" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J24" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80480_lancashire", ".\export_data\inspection_reports\80480_lancashire")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80478_kirklees", ".\export_data\inspection_reports\80478_kirklees")</f>
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L24" t="s">
         <v>9</v>
@@ -3315,7 +3348,7 @@
         <v>9</v>
       </c>
       <c r="N24" t="s">
-        <v>259</v>
+        <v>9</v>
       </c>
       <c r="O24" t="s">
         <v>260</v>
@@ -3338,7 +3371,7 @@
         <v>263</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
         <v>264</v>
@@ -3353,17 +3386,17 @@
         <v>267</v>
       </c>
       <c r="H25" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="I25" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="J25" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80481_leeds", ".\export_data\inspection_reports\80481_leeds")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80480_lancashire", ".\export_data\inspection_reports\80480_lancashire")</f>
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L25" t="s">
         <v>9</v>
@@ -3372,13 +3405,13 @@
         <v>9</v>
       </c>
       <c r="N25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="O25" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="P25" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Q25" t="s">
         <v>12</v>
@@ -3389,184 +3422,184 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E26" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H26" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="I26" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80481_leeds", ".\export_data\inspection_reports\80481_leeds")</f>
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
         <v>279</v>
       </c>
-      <c r="J26" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80484_lincolnshire", ".\export_data\inspection_reports\80484_lincolnshire")</f>
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" t="s">
         <v>280</v>
       </c>
-      <c r="L26" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>281</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>282</v>
       </c>
-      <c r="O26" t="s">
-        <v>9</v>
-      </c>
-      <c r="P26" t="s">
-        <v>9</v>
-      </c>
       <c r="Q26" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R26" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" t="s">
         <v>284</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" t="s">
         <v>285</v>
       </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>286</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>287</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" t="s">
         <v>289</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>290</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80484_lincolnshire", ".\export_data\inspection_reports\80484_lincolnshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
         <v>291</v>
       </c>
-      <c r="J27" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80485_liverpool", ".\export_data\inspection_reports\80485_liverpool")</f>
-        <v>0</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" t="s">
         <v>292</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>293</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
+        <v>9</v>
+      </c>
+      <c r="P27" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>82</v>
+      </c>
+      <c r="R27" t="s">
         <v>294</v>
-      </c>
-      <c r="N27" t="s">
-        <v>295</v>
-      </c>
-      <c r="O27" t="s">
-        <v>9</v>
-      </c>
-      <c r="P27" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>296</v>
-      </c>
-      <c r="R27" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>297</v>
+      </c>
+      <c r="E28" t="s">
         <v>298</v>
       </c>
-      <c r="B28" t="s">
+      <c r="F28" t="s">
         <v>299</v>
       </c>
-      <c r="C28" t="s">
+      <c r="G28" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" t="s">
         <v>301</v>
       </c>
-      <c r="E28" t="s">
+      <c r="I28" t="s">
         <v>302</v>
       </c>
-      <c r="F28" t="s">
+      <c r="J28" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80485_liverpool", ".\export_data\inspection_reports\80485_liverpool")</f>
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
         <v>303</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="L28" t="s">
         <v>304</v>
       </c>
-      <c r="H28" t="s">
+      <c r="M28" t="s">
         <v>305</v>
       </c>
-      <c r="I28" t="s">
-        <v>305</v>
-      </c>
-      <c r="J28" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80488_bexley", ".\export_data\inspection_reports\80488_bexley")</f>
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="N28" t="s">
         <v>306</v>
       </c>
-      <c r="L28" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" t="s">
         <v>307</v>
       </c>
-      <c r="N28" t="s">
+      <c r="R28" t="s">
         <v>308</v>
-      </c>
-      <c r="O28" t="s">
-        <v>9</v>
-      </c>
-      <c r="P28" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>71</v>
-      </c>
-      <c r="R28" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" t="s">
+        <v>309</v>
+      </c>
+      <c r="B29" t="s">
         <v>310</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>311</v>
-      </c>
-      <c r="C29" t="s">
-        <v>300</v>
       </c>
       <c r="D29" t="s">
         <v>312</v>
@@ -3587,7 +3620,7 @@
         <v>316</v>
       </c>
       <c r="J29" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80490_bromley", ".\export_data\inspection_reports\80490_bromley")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80488_bexley", ".\export_data\inspection_reports\80488_bexley")</f>
         <v>0</v>
       </c>
       <c r="K29" t="s">
@@ -3597,22 +3630,22 @@
         <v>9</v>
       </c>
       <c r="M29" t="s">
-        <v>9</v>
+        <v>318</v>
       </c>
       <c r="N29" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O29" t="s">
-        <v>319</v>
+        <v>9</v>
       </c>
       <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>82</v>
+      </c>
+      <c r="R29" t="s">
         <v>320</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>12</v>
-      </c>
-      <c r="R29" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -3623,7 +3656,7 @@
         <v>322</v>
       </c>
       <c r="C30" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D30" t="s">
         <v>323</v>
@@ -3644,7 +3677,7 @@
         <v>327</v>
       </c>
       <c r="J30" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80492_croydon", ".\export_data\inspection_reports\80492_croydon")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80490_bromley", ".\export_data\inspection_reports\80490_bromley")</f>
         <v>0</v>
       </c>
       <c r="K30" t="s">
@@ -3654,22 +3687,22 @@
         <v>9</v>
       </c>
       <c r="M30" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" t="s">
         <v>329</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>330</v>
       </c>
-      <c r="O30" t="s">
-        <v>9</v>
-      </c>
       <c r="P30" t="s">
-        <v>9</v>
+        <v>331</v>
       </c>
       <c r="Q30" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R30" t="s">
-        <v>331</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -3680,7 +3713,7 @@
         <v>333</v>
       </c>
       <c r="C31" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D31" t="s">
         <v>334</v>
@@ -3701,7 +3734,7 @@
         <v>338</v>
       </c>
       <c r="J31" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80495_greenwich", ".\export_data\inspection_reports\80495_greenwich")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80492_croydon", ".\export_data\inspection_reports\80492_croydon")</f>
         <v>0</v>
       </c>
       <c r="K31" t="s">
@@ -3723,7 +3756,7 @@
         <v>9</v>
       </c>
       <c r="Q31" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R31" t="s">
         <v>342</v>
@@ -3737,7 +3770,7 @@
         <v>344</v>
       </c>
       <c r="C32" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
         <v>345</v>
@@ -3758,7 +3791,7 @@
         <v>349</v>
       </c>
       <c r="J32" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80498_haringey", ".\export_data\inspection_reports\80498_haringey")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80495_greenwich", ".\export_data\inspection_reports\80495_greenwich")</f>
         <v>0</v>
       </c>
       <c r="K32" t="s">
@@ -3780,7 +3813,7 @@
         <v>9</v>
       </c>
       <c r="Q32" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R32" t="s">
         <v>353</v>
@@ -3794,7 +3827,7 @@
         <v>355</v>
       </c>
       <c r="C33" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D33" t="s">
         <v>356</v>
@@ -3815,7 +3848,7 @@
         <v>360</v>
       </c>
       <c r="J33" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80499_harrow", ".\export_data\inspection_reports\80499_harrow")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80498_haringey", ".\export_data\inspection_reports\80498_haringey")</f>
         <v>0</v>
       </c>
       <c r="K33" t="s">
@@ -3825,22 +3858,22 @@
         <v>9</v>
       </c>
       <c r="M33" t="s">
-        <v>9</v>
+        <v>362</v>
       </c>
       <c r="N33" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="O33" t="s">
-        <v>363</v>
+        <v>9</v>
       </c>
       <c r="P33" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>82</v>
+      </c>
+      <c r="R33" t="s">
         <v>364</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>12</v>
-      </c>
-      <c r="R33" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -3851,7 +3884,7 @@
         <v>366</v>
       </c>
       <c r="C34" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
         <v>367</v>
@@ -3872,7 +3905,7 @@
         <v>371</v>
       </c>
       <c r="J34" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80501_hillingdon", ".\export_data\inspection_reports\80501_hillingdon")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80499_harrow", ".\export_data\inspection_reports\80499_harrow")</f>
         <v>0</v>
       </c>
       <c r="K34" t="s">
@@ -3908,7 +3941,7 @@
         <v>377</v>
       </c>
       <c r="C35" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D35" t="s">
         <v>378</v>
@@ -3929,7 +3962,7 @@
         <v>382</v>
       </c>
       <c r="J35" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80501_hillingdon", ".\export_data\inspection_reports\80501_hillingdon")</f>
         <v>0</v>
       </c>
       <c r="K35" t="s">
@@ -3939,22 +3972,22 @@
         <v>9</v>
       </c>
       <c r="M35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" t="s">
         <v>384</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>385</v>
       </c>
-      <c r="O35" t="s">
-        <v>9</v>
-      </c>
       <c r="P35" t="s">
-        <v>9</v>
+        <v>386</v>
       </c>
       <c r="Q35" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="R35" t="s">
-        <v>386</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -3965,7 +3998,7 @@
         <v>388</v>
       </c>
       <c r="C36" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D36" t="s">
         <v>389</v>
@@ -3986,7 +4019,7 @@
         <v>393</v>
       </c>
       <c r="J36" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
         <v>0</v>
       </c>
       <c r="K36" t="s">
@@ -4008,61 +4041,61 @@
         <v>9</v>
       </c>
       <c r="Q36" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="R36" t="s">
-        <v>9</v>
+        <v>397</v>
       </c>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B37" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C37" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D37" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E37" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F37" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H37" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I37" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="J37" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
         <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L37" t="s">
         <v>9</v>
       </c>
       <c r="M37" t="s">
-        <v>9</v>
+        <v>406</v>
       </c>
       <c r="N37" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="O37" t="s">
-        <v>406</v>
+        <v>9</v>
       </c>
       <c r="P37" t="s">
-        <v>407</v>
+        <v>9</v>
       </c>
       <c r="Q37" t="s">
         <v>12</v>
@@ -4079,7 +4112,7 @@
         <v>409</v>
       </c>
       <c r="C38" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D38" t="s">
         <v>410</v>
@@ -4100,7 +4133,7 @@
         <v>414</v>
       </c>
       <c r="J38" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
         <v>0</v>
       </c>
       <c r="K38" t="s">
@@ -4136,7 +4169,7 @@
         <v>420</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D39" t="s">
         <v>421</v>
@@ -4157,7 +4190,7 @@
         <v>425</v>
       </c>
       <c r="J39" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
         <v>0</v>
       </c>
       <c r="K39" t="s">
@@ -4193,7 +4226,7 @@
         <v>431</v>
       </c>
       <c r="C40" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="D40" t="s">
         <v>432</v>
@@ -4214,7 +4247,7 @@
         <v>436</v>
       </c>
       <c r="J40" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
         <v>0</v>
       </c>
       <c r="K40" t="s">
@@ -4250,7 +4283,7 @@
         <v>442</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>311</v>
       </c>
       <c r="D41" t="s">
         <v>443</v>
@@ -4271,7 +4304,7 @@
         <v>447</v>
       </c>
       <c r="J41" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
         <v>0</v>
       </c>
       <c r="K41" t="s">
@@ -4307,107 +4340,107 @@
         <v>453</v>
       </c>
       <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
         <v>454</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>455</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>456</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" t="s">
         <v>458</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
+        <v>458</v>
+      </c>
+      <c r="J42" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
         <v>459</v>
       </c>
-      <c r="I42" t="s">
-        <v>459</v>
-      </c>
-      <c r="J42" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" t="s">
         <v>460</v>
       </c>
-      <c r="L42" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="O42" t="s">
         <v>461</v>
       </c>
-      <c r="N42" t="s">
+      <c r="P42" t="s">
         <v>462</v>
       </c>
-      <c r="O42" t="s">
-        <v>9</v>
-      </c>
-      <c r="P42" t="s">
-        <v>9</v>
-      </c>
       <c r="Q42" t="s">
-        <v>463</v>
+        <v>12</v>
       </c>
       <c r="R42" t="s">
-        <v>464</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:18">
       <c r="A43" t="s">
+        <v>463</v>
+      </c>
+      <c r="B43" t="s">
+        <v>464</v>
+      </c>
+      <c r="C43" t="s">
         <v>465</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>466</v>
       </c>
-      <c r="C43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>467</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>468</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" t="s">
         <v>470</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
+        <v>470</v>
+      </c>
+      <c r="J43" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
         <v>471</v>
       </c>
-      <c r="I43" t="s">
-        <v>471</v>
-      </c>
-      <c r="J43" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
-        <v>0</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" t="s">
         <v>472</v>
       </c>
-      <c r="L43" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>473</v>
       </c>
-      <c r="N43" t="s">
+      <c r="O43" t="s">
+        <v>9</v>
+      </c>
+      <c r="P43" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" t="s">
         <v>474</v>
-      </c>
-      <c r="O43" t="s">
-        <v>9</v>
-      </c>
-      <c r="P43" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>71</v>
       </c>
       <c r="R43" t="s">
         <v>475</v>
@@ -4421,7 +4454,7 @@
         <v>477</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
         <v>478</v>
@@ -4442,7 +4475,7 @@
         <v>482</v>
       </c>
       <c r="J44" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
         <v>0</v>
       </c>
       <c r="K44" t="s">
@@ -4452,22 +4485,22 @@
         <v>9</v>
       </c>
       <c r="M44" t="s">
-        <v>9</v>
+        <v>484</v>
       </c>
       <c r="N44" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="O44" t="s">
-        <v>485</v>
+        <v>9</v>
       </c>
       <c r="P44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>82</v>
+      </c>
+      <c r="R44" t="s">
         <v>486</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>12</v>
-      </c>
-      <c r="R44" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -4478,7 +4511,7 @@
         <v>488</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
         <v>489</v>
@@ -4499,7 +4532,7 @@
         <v>493</v>
       </c>
       <c r="J45" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
         <v>0</v>
       </c>
       <c r="K45" t="s">
@@ -4535,7 +4568,7 @@
         <v>499</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
         <v>500</v>
@@ -4556,32 +4589,89 @@
         <v>504</v>
       </c>
       <c r="J46" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
+        <v>505</v>
+      </c>
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" t="s">
+        <v>506</v>
+      </c>
+      <c r="O46" t="s">
+        <v>507</v>
+      </c>
+      <c r="P46" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>12</v>
+      </c>
+      <c r="R46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" t="s">
+        <v>509</v>
+      </c>
+      <c r="B47" t="s">
+        <v>510</v>
+      </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" t="s">
+        <v>511</v>
+      </c>
+      <c r="E47" t="s">
+        <v>512</v>
+      </c>
+      <c r="F47" t="s">
+        <v>513</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H47" t="s">
+        <v>515</v>
+      </c>
+      <c r="I47" t="s">
+        <v>515</v>
+      </c>
+      <c r="J47" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80532_northumberland", ".\export_data\inspection_reports\80532_northumberland")</f>
         <v>0</v>
       </c>
-      <c r="K46" t="s">
-        <v>505</v>
-      </c>
-      <c r="L46" t="s">
-        <v>9</v>
-      </c>
-      <c r="M46" t="s">
-        <v>506</v>
-      </c>
-      <c r="N46" t="s">
-        <v>507</v>
-      </c>
-      <c r="O46" t="s">
-        <v>9</v>
-      </c>
-      <c r="P46" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>71</v>
-      </c>
-      <c r="R46" t="s">
-        <v>508</v>
+      <c r="K47" t="s">
+        <v>516</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>517</v>
+      </c>
+      <c r="N47" t="s">
+        <v>518</v>
+      </c>
+      <c r="O47" t="s">
+        <v>9</v>
+      </c>
+      <c r="P47" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>82</v>
+      </c>
+      <c r="R47" t="s">
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -4631,6 +4721,7 @@
     <hyperlink ref="G44" r:id="rId43"/>
     <hyperlink ref="G45" r:id="rId44"/>
     <hyperlink ref="G46" r:id="rId45"/>
+    <hyperlink ref="G47" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
JTAI refresh, 2026-02-16 05:34:09
</commit_message>
<xml_diff>
--- a/ofsted_csc_jtai_overview.xlsx
+++ b/ofsted_csc_jtai_overview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="548">
   <si>
     <t>80426</t>
   </si>
@@ -863,6 +863,36 @@
   </si>
   <si>
     <t>Consistent and timely sharing of police protection notifications (PPNs) when police officers identify risks to children. The quality of PPNs should include detailed information, including a childs ethnicity and culture, to assist with multi- agency decision-making. Waiting times for children to receive CAMHS assessments and therapeutic treatment in line with needs arising from their mental health conditions and neurodiversity.</t>
+  </si>
+  <si>
+    <t>80483</t>
+  </si>
+  <si>
+    <t>855</t>
+  </si>
+  <si>
+    <t>E10000018</t>
+  </si>
+  <si>
+    <t>916, 803, 937, 802, 850, 865, 933, 938, 811, 891</t>
+  </si>
+  <si>
+    <t>leicestershire</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50295353</t>
+  </si>
+  <si>
+    <t>12/02/26</t>
+  </si>
+  <si>
+    <t>Child sexual abuse in the family environment in leicestershire.</t>
+  </si>
+  <si>
+    <t>The partnership in Leicestershire has prioritised and is working to strengthen their understanding of Child Sexual Abuse in the Family Environment (CSAFE), with regular reviews of key achievements through an agreed action plan. Although the partnerships strategy is still in draft form, its ambition is evident through collaboration with the National Society for Prevention of Cruelty to Children (NSPCC) and the Centre of Expertise in Child Sexual Abuse (CSA Centre). The strategy has also drawn helpful insights from local safeguarding practice reviews, thematic briefings, surveys and audits to inform planning and practice.</t>
+  </si>
+  <si>
+    <t>Improve information-sharing across the partnership, especially at the initial contact and referral stage. While thresholds are appropriate, not all relevant details are consistently shared early on, limiting the effectiveness of risk assessments. Timeliness of child protection processes, particularly strategy meetings and initial child protection conferences, and sharing of minutes of these multi-agency meetings.</t>
   </si>
   <si>
     <t>80484</t>
@@ -1990,7 +2020,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1998,58 +2028,58 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>526</v>
+        <v>536</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>537</v>
+        <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -3503,308 +3533,308 @@
         <v>289</v>
       </c>
       <c r="I27" t="s">
+        <v>289</v>
+      </c>
+      <c r="J27" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80483_leicestershire", ".\export_data\inspection_reports\80483_leicestershire")</f>
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
         <v>290</v>
       </c>
-      <c r="J27" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80484_lincolnshire", ".\export_data\inspection_reports\80484_lincolnshire")</f>
-        <v>0</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" t="s">
+        <v>68</v>
+      </c>
+      <c r="O27" t="s">
         <v>291</v>
       </c>
-      <c r="L27" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="P27" t="s">
         <v>292</v>
       </c>
-      <c r="N27" t="s">
-        <v>293</v>
-      </c>
-      <c r="O27" t="s">
-        <v>9</v>
-      </c>
-      <c r="P27" t="s">
-        <v>9</v>
-      </c>
       <c r="Q27" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="R27" t="s">
-        <v>294</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" t="s">
         <v>295</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E28" t="s">
         <v>296</v>
       </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>297</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>299</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="I28" t="s">
         <v>300</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80484_lincolnshire", ".\export_data\inspection_reports\80484_lincolnshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
         <v>301</v>
       </c>
-      <c r="I28" t="s">
+      <c r="L28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" t="s">
         <v>302</v>
       </c>
-      <c r="J28" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80485_liverpool", ".\export_data\inspection_reports\80485_liverpool")</f>
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="N28" t="s">
         <v>303</v>
       </c>
-      <c r="L28" t="s">
+      <c r="O28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>82</v>
+      </c>
+      <c r="R28" t="s">
         <v>304</v>
-      </c>
-      <c r="M28" t="s">
-        <v>305</v>
-      </c>
-      <c r="N28" t="s">
-        <v>306</v>
-      </c>
-      <c r="O28" t="s">
-        <v>9</v>
-      </c>
-      <c r="P28" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>307</v>
-      </c>
-      <c r="R28" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" t="s">
+        <v>306</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>307</v>
+      </c>
+      <c r="E29" t="s">
+        <v>308</v>
+      </c>
+      <c r="F29" t="s">
         <v>309</v>
       </c>
-      <c r="B29" t="s">
+      <c r="G29" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C29" t="s">
+      <c r="H29" t="s">
         <v>311</v>
       </c>
-      <c r="D29" t="s">
+      <c r="I29" t="s">
         <v>312</v>
       </c>
-      <c r="E29" t="s">
+      <c r="J29" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80485_liverpool", ".\export_data\inspection_reports\80485_liverpool")</f>
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
         <v>313</v>
       </c>
-      <c r="F29" t="s">
+      <c r="L29" t="s">
         <v>314</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="M29" t="s">
         <v>315</v>
       </c>
-      <c r="H29" t="s">
+      <c r="N29" t="s">
         <v>316</v>
       </c>
-      <c r="I29" t="s">
-        <v>316</v>
-      </c>
-      <c r="J29" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80488_bexley", ".\export_data\inspection_reports\80488_bexley")</f>
-        <v>0</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="O29" t="s">
+        <v>9</v>
+      </c>
+      <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
         <v>317</v>
       </c>
-      <c r="L29" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" t="s">
+      <c r="R29" t="s">
         <v>318</v>
-      </c>
-      <c r="N29" t="s">
-        <v>319</v>
-      </c>
-      <c r="O29" t="s">
-        <v>9</v>
-      </c>
-      <c r="P29" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>82</v>
-      </c>
-      <c r="R29" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
+        <v>319</v>
+      </c>
+      <c r="B30" t="s">
+        <v>320</v>
+      </c>
+      <c r="C30" t="s">
         <v>321</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>322</v>
       </c>
-      <c r="C30" t="s">
-        <v>311</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>323</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>324</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" t="s">
         <v>326</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
+        <v>326</v>
+      </c>
+      <c r="J30" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80488_bexley", ".\export_data\inspection_reports\80488_bexley")</f>
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
         <v>327</v>
       </c>
-      <c r="I30" t="s">
-        <v>327</v>
-      </c>
-      <c r="J30" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80490_bromley", ".\export_data\inspection_reports\80490_bromley")</f>
-        <v>0</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" t="s">
         <v>328</v>
-      </c>
-      <c r="L30" t="s">
-        <v>9</v>
-      </c>
-      <c r="M30" t="s">
-        <v>9</v>
       </c>
       <c r="N30" t="s">
         <v>329</v>
       </c>
       <c r="O30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>82</v>
+      </c>
+      <c r="R30" t="s">
         <v>330</v>
-      </c>
-      <c r="P30" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>12</v>
-      </c>
-      <c r="R30" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
+        <v>331</v>
+      </c>
+      <c r="B31" t="s">
         <v>332</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>321</v>
+      </c>
+      <c r="D31" t="s">
         <v>333</v>
       </c>
-      <c r="C31" t="s">
-        <v>311</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>334</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>335</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" t="s">
         <v>337</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
+        <v>337</v>
+      </c>
+      <c r="J31" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80490_bromley", ".\export_data\inspection_reports\80490_bromley")</f>
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
         <v>338</v>
       </c>
-      <c r="I31" t="s">
-        <v>338</v>
-      </c>
-      <c r="J31" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80492_croydon", ".\export_data\inspection_reports\80492_croydon")</f>
-        <v>0</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" t="s">
+        <v>9</v>
+      </c>
+      <c r="N31" t="s">
         <v>339</v>
       </c>
-      <c r="L31" t="s">
-        <v>9</v>
-      </c>
-      <c r="M31" t="s">
+      <c r="O31" t="s">
         <v>340</v>
       </c>
-      <c r="N31" t="s">
+      <c r="P31" t="s">
         <v>341</v>
       </c>
-      <c r="O31" t="s">
-        <v>9</v>
-      </c>
-      <c r="P31" t="s">
-        <v>9</v>
-      </c>
       <c r="Q31" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="R31" t="s">
-        <v>342</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
+        <v>342</v>
+      </c>
+      <c r="B32" t="s">
         <v>343</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>321</v>
+      </c>
+      <c r="D32" t="s">
         <v>344</v>
       </c>
-      <c r="C32" t="s">
-        <v>311</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>345</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>346</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" t="s">
         <v>348</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
+        <v>348</v>
+      </c>
+      <c r="J32" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80492_croydon", ".\export_data\inspection_reports\80492_croydon")</f>
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
         <v>349</v>
       </c>
-      <c r="I32" t="s">
-        <v>349</v>
-      </c>
-      <c r="J32" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80495_greenwich", ".\export_data\inspection_reports\80495_greenwich")</f>
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" t="s">
         <v>350</v>
       </c>
-      <c r="L32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>351</v>
-      </c>
-      <c r="N32" t="s">
-        <v>352</v>
       </c>
       <c r="O32" t="s">
         <v>9</v>
@@ -3816,52 +3846,52 @@
         <v>82</v>
       </c>
       <c r="R32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
+        <v>353</v>
+      </c>
+      <c r="B33" t="s">
         <v>354</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>321</v>
+      </c>
+      <c r="D33" t="s">
         <v>355</v>
       </c>
-      <c r="C33" t="s">
-        <v>311</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>356</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>357</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" t="s">
         <v>359</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
+        <v>359</v>
+      </c>
+      <c r="J33" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80495_greenwich", ".\export_data\inspection_reports\80495_greenwich")</f>
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
         <v>360</v>
       </c>
-      <c r="I33" t="s">
-        <v>360</v>
-      </c>
-      <c r="J33" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80498_haringey", ".\export_data\inspection_reports\80498_haringey")</f>
-        <v>0</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" t="s">
         <v>361</v>
       </c>
-      <c r="L33" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>362</v>
-      </c>
-      <c r="N33" t="s">
-        <v>363</v>
       </c>
       <c r="O33" t="s">
         <v>9</v>
@@ -3873,115 +3903,115 @@
         <v>82</v>
       </c>
       <c r="R33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
+        <v>364</v>
+      </c>
+      <c r="B34" t="s">
         <v>365</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>321</v>
+      </c>
+      <c r="D34" t="s">
         <v>366</v>
       </c>
-      <c r="C34" t="s">
-        <v>311</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>367</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>368</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" t="s">
         <v>370</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
+        <v>370</v>
+      </c>
+      <c r="J34" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80498_haringey", ".\export_data\inspection_reports\80498_haringey")</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
         <v>371</v>
       </c>
-      <c r="I34" t="s">
-        <v>371</v>
-      </c>
-      <c r="J34" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80499_harrow", ".\export_data\inspection_reports\80499_harrow")</f>
-        <v>0</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" t="s">
         <v>372</v>
-      </c>
-      <c r="L34" t="s">
-        <v>9</v>
-      </c>
-      <c r="M34" t="s">
-        <v>9</v>
       </c>
       <c r="N34" t="s">
         <v>373</v>
       </c>
       <c r="O34" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R34" t="s">
         <v>374</v>
-      </c>
-      <c r="P34" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>12</v>
-      </c>
-      <c r="R34" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" t="s">
+        <v>375</v>
+      </c>
+      <c r="B35" t="s">
         <v>376</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>321</v>
+      </c>
+      <c r="D35" t="s">
         <v>377</v>
       </c>
-      <c r="C35" t="s">
-        <v>311</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>378</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>379</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" t="s">
         <v>381</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
+        <v>381</v>
+      </c>
+      <c r="J35" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80499_harrow", ".\export_data\inspection_reports\80499_harrow")</f>
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
         <v>382</v>
       </c>
-      <c r="I35" t="s">
-        <v>382</v>
-      </c>
-      <c r="J35" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80501_hillingdon", ".\export_data\inspection_reports\80501_hillingdon")</f>
-        <v>0</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" t="s">
         <v>383</v>
       </c>
-      <c r="L35" t="s">
-        <v>9</v>
-      </c>
-      <c r="M35" t="s">
-        <v>9</v>
-      </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>384</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>385</v>
-      </c>
-      <c r="P35" t="s">
-        <v>386</v>
       </c>
       <c r="Q35" t="s">
         <v>12</v>
@@ -3992,116 +4022,116 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" t="s">
+        <v>386</v>
+      </c>
+      <c r="B36" t="s">
         <v>387</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>321</v>
+      </c>
+      <c r="D36" t="s">
         <v>388</v>
       </c>
-      <c r="C36" t="s">
-        <v>311</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>389</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>390</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" t="s">
         <v>392</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
+        <v>392</v>
+      </c>
+      <c r="J36" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80501_hillingdon", ".\export_data\inspection_reports\80501_hillingdon")</f>
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
         <v>393</v>
       </c>
-      <c r="I36" t="s">
-        <v>393</v>
-      </c>
-      <c r="J36" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" t="s">
         <v>394</v>
       </c>
-      <c r="L36" t="s">
-        <v>9</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="O36" t="s">
         <v>395</v>
       </c>
-      <c r="N36" t="s">
+      <c r="P36" t="s">
         <v>396</v>
       </c>
-      <c r="O36" t="s">
-        <v>9</v>
-      </c>
-      <c r="P36" t="s">
-        <v>9</v>
-      </c>
       <c r="Q36" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="R36" t="s">
-        <v>397</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" t="s">
+        <v>397</v>
+      </c>
+      <c r="B37" t="s">
         <v>398</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" t="s">
         <v>399</v>
       </c>
-      <c r="C37" t="s">
-        <v>311</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>400</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>401</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" t="s">
         <v>403</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
+        <v>403</v>
+      </c>
+      <c r="J37" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80503_hounslow", ".\export_data\inspection_reports\80503_hounslow")</f>
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
         <v>404</v>
       </c>
-      <c r="I37" t="s">
-        <v>404</v>
-      </c>
-      <c r="J37" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
-        <v>0</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" t="s">
         <v>405</v>
       </c>
-      <c r="L37" t="s">
-        <v>9</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>406</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" t="s">
         <v>407</v>
-      </c>
-      <c r="O37" t="s">
-        <v>9</v>
-      </c>
-      <c r="P37" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>12</v>
-      </c>
-      <c r="R37" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -4112,7 +4142,7 @@
         <v>409</v>
       </c>
       <c r="C38" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="D38" t="s">
         <v>410</v>
@@ -4133,7 +4163,7 @@
         <v>414</v>
       </c>
       <c r="J38" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80505_islington", ".\export_data\inspection_reports\80505_islington")</f>
         <v>0</v>
       </c>
       <c r="K38" t="s">
@@ -4143,16 +4173,16 @@
         <v>9</v>
       </c>
       <c r="M38" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="N38" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="O38" t="s">
-        <v>417</v>
+        <v>9</v>
       </c>
       <c r="P38" t="s">
-        <v>418</v>
+        <v>9</v>
       </c>
       <c r="Q38" t="s">
         <v>12</v>
@@ -4163,53 +4193,53 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" t="s">
+        <v>418</v>
+      </c>
+      <c r="B39" t="s">
         <v>419</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>321</v>
+      </c>
+      <c r="D39" t="s">
         <v>420</v>
       </c>
-      <c r="C39" t="s">
-        <v>311</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>421</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>422</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" t="s">
         <v>424</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
+        <v>424</v>
+      </c>
+      <c r="J39" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80508_lewisham", ".\export_data\inspection_reports\80508_lewisham")</f>
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
         <v>425</v>
       </c>
-      <c r="I39" t="s">
-        <v>425</v>
-      </c>
-      <c r="J39" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
-        <v>0</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" t="s">
+        <v>9</v>
+      </c>
+      <c r="N39" t="s">
         <v>426</v>
       </c>
-      <c r="L39" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" t="s">
-        <v>9</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>427</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>428</v>
-      </c>
-      <c r="P39" t="s">
-        <v>429</v>
       </c>
       <c r="Q39" t="s">
         <v>12</v>
@@ -4220,53 +4250,53 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" t="s">
+        <v>429</v>
+      </c>
+      <c r="B40" t="s">
         <v>430</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>321</v>
+      </c>
+      <c r="D40" t="s">
         <v>431</v>
       </c>
-      <c r="C40" t="s">
-        <v>311</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>432</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>433</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" t="s">
         <v>435</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
+        <v>435</v>
+      </c>
+      <c r="J40" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80510_merton", ".\export_data\inspection_reports\80510_merton")</f>
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
         <v>436</v>
       </c>
-      <c r="I40" t="s">
-        <v>436</v>
-      </c>
-      <c r="J40" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
-        <v>0</v>
-      </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" t="s">
         <v>437</v>
       </c>
-      <c r="L40" t="s">
-        <v>9</v>
-      </c>
-      <c r="M40" t="s">
-        <v>9</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>438</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>439</v>
-      </c>
-      <c r="P40" t="s">
-        <v>440</v>
       </c>
       <c r="Q40" t="s">
         <v>12</v>
@@ -4277,53 +4307,53 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" t="s">
+        <v>440</v>
+      </c>
+      <c r="B41" t="s">
         <v>441</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>321</v>
+      </c>
+      <c r="D41" t="s">
         <v>442</v>
       </c>
-      <c r="C41" t="s">
-        <v>311</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>443</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>444</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" t="s">
         <v>446</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
+        <v>446</v>
+      </c>
+      <c r="J41" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80513_richmond upon thames", ".\export_data\inspection_reports\80513_richmond upon thames")</f>
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
         <v>447</v>
       </c>
-      <c r="I41" t="s">
-        <v>447</v>
-      </c>
-      <c r="J41" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
-        <v>0</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" t="s">
         <v>448</v>
       </c>
-      <c r="L41" t="s">
-        <v>9</v>
-      </c>
-      <c r="M41" t="s">
-        <v>9</v>
-      </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>449</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>450</v>
-      </c>
-      <c r="P41" t="s">
-        <v>451</v>
       </c>
       <c r="Q41" t="s">
         <v>12</v>
@@ -4334,53 +4364,53 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" t="s">
+        <v>451</v>
+      </c>
+      <c r="B42" t="s">
         <v>452</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>321</v>
+      </c>
+      <c r="D42" t="s">
         <v>453</v>
       </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>454</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>455</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" t="s">
         <v>457</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
+        <v>457</v>
+      </c>
+      <c r="J42" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80515_sutton", ".\export_data\inspection_reports\80515_sutton")</f>
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
         <v>458</v>
       </c>
-      <c r="I42" t="s">
-        <v>458</v>
-      </c>
-      <c r="J42" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" t="s">
         <v>459</v>
       </c>
-      <c r="L42" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" t="s">
-        <v>9</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
         <v>460</v>
       </c>
-      <c r="O42" t="s">
+      <c r="P42" t="s">
         <v>461</v>
-      </c>
-      <c r="P42" t="s">
-        <v>462</v>
       </c>
       <c r="Q42" t="s">
         <v>12</v>
@@ -4391,224 +4421,224 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" t="s">
+        <v>462</v>
+      </c>
+      <c r="B43" t="s">
         <v>463</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
         <v>464</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
         <v>465</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
         <v>466</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="F43" t="s">
+      <c r="H43" t="s">
         <v>468</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="I43" t="s">
+        <v>468</v>
+      </c>
+      <c r="J43" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80521_manchester", ".\export_data\inspection_reports\80521_manchester")</f>
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
         <v>469</v>
       </c>
-      <c r="H43" t="s">
+      <c r="L43" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43" t="s">
         <v>470</v>
       </c>
-      <c r="I43" t="s">
-        <v>470</v>
-      </c>
-      <c r="J43" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
-        <v>0</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="O43" t="s">
         <v>471</v>
       </c>
-      <c r="L43" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="P43" t="s">
         <v>472</v>
       </c>
-      <c r="N43" t="s">
-        <v>473</v>
-      </c>
-      <c r="O43" t="s">
-        <v>9</v>
-      </c>
-      <c r="P43" t="s">
-        <v>9</v>
-      </c>
       <c r="Q43" t="s">
-        <v>474</v>
+        <v>12</v>
       </c>
       <c r="R43" t="s">
-        <v>475</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:18">
       <c r="A44" t="s">
+        <v>473</v>
+      </c>
+      <c r="B44" t="s">
+        <v>474</v>
+      </c>
+      <c r="C44" t="s">
+        <v>475</v>
+      </c>
+      <c r="D44" t="s">
         <v>476</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
         <v>477</v>
       </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="F44" t="s">
         <v>478</v>
       </c>
-      <c r="E44" t="s">
+      <c r="G44" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
         <v>480</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="I44" t="s">
+        <v>480</v>
+      </c>
+      <c r="J44" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80522_medway", ".\export_data\inspection_reports\80522_medway")</f>
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
         <v>481</v>
       </c>
-      <c r="H44" t="s">
+      <c r="L44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" t="s">
         <v>482</v>
       </c>
-      <c r="I44" t="s">
-        <v>482</v>
-      </c>
-      <c r="J44" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
-        <v>0</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="N44" t="s">
         <v>483</v>
       </c>
-      <c r="L44" t="s">
-        <v>9</v>
-      </c>
-      <c r="M44" t="s">
+      <c r="O44" t="s">
+        <v>9</v>
+      </c>
+      <c r="P44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" t="s">
         <v>484</v>
       </c>
-      <c r="N44" t="s">
+      <c r="R44" t="s">
         <v>485</v>
-      </c>
-      <c r="O44" t="s">
-        <v>9</v>
-      </c>
-      <c r="P44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>82</v>
-      </c>
-      <c r="R44" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" t="s">
+        <v>486</v>
+      </c>
+      <c r="B45" t="s">
         <v>487</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
         <v>488</v>
       </c>
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>489</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>490</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" t="s">
         <v>492</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
+        <v>492</v>
+      </c>
+      <c r="J45" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80524_milton keynes", ".\export_data\inspection_reports\80524_milton keynes")</f>
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
         <v>493</v>
       </c>
-      <c r="I45" t="s">
-        <v>493</v>
-      </c>
-      <c r="J45" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
-        <v>0</v>
-      </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" t="s">
         <v>494</v>
-      </c>
-      <c r="L45" t="s">
-        <v>9</v>
-      </c>
-      <c r="M45" t="s">
-        <v>9</v>
       </c>
       <c r="N45" t="s">
         <v>495</v>
       </c>
       <c r="O45" t="s">
+        <v>9</v>
+      </c>
+      <c r="P45" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>82</v>
+      </c>
+      <c r="R45" t="s">
         <v>496</v>
-      </c>
-      <c r="P45" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>12</v>
-      </c>
-      <c r="R45" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="A46" t="s">
+        <v>497</v>
+      </c>
+      <c r="B46" t="s">
         <v>498</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
         <v>499</v>
       </c>
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>500</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>501</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" t="s">
         <v>503</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
+        <v>503</v>
+      </c>
+      <c r="J46" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80418_norfolk", ".\export_data\inspection_reports\80418_norfolk")</f>
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
         <v>504</v>
       </c>
-      <c r="I46" t="s">
-        <v>504</v>
-      </c>
-      <c r="J46" s="3">
-        <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
-        <v>0</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" t="s">
         <v>505</v>
       </c>
-      <c r="L46" t="s">
-        <v>9</v>
-      </c>
-      <c r="M46" t="s">
-        <v>9</v>
-      </c>
-      <c r="N46" t="s">
+      <c r="O46" t="s">
         <v>506</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>507</v>
-      </c>
-      <c r="P46" t="s">
-        <v>508</v>
       </c>
       <c r="Q46" t="s">
         <v>12</v>
@@ -4619,59 +4649,116 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" t="s">
+        <v>508</v>
+      </c>
+      <c r="B47" t="s">
         <v>509</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
         <v>510</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
+        <v>511</v>
+      </c>
+      <c r="F47" t="s">
+        <v>512</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="H47" t="s">
+        <v>514</v>
+      </c>
+      <c r="I47" t="s">
+        <v>514</v>
+      </c>
+      <c r="J47" s="3">
+        <f>HYPERLINK(".\.\export_data\inspection_reports\80530_north yorkshire", ".\export_data\inspection_reports\80530_north yorkshire")</f>
+        <v>0</v>
+      </c>
+      <c r="K47" t="s">
+        <v>515</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>9</v>
+      </c>
+      <c r="N47" t="s">
+        <v>516</v>
+      </c>
+      <c r="O47" t="s">
+        <v>517</v>
+      </c>
+      <c r="P47" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>12</v>
+      </c>
+      <c r="R47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" t="s">
+        <v>519</v>
+      </c>
+      <c r="B48" t="s">
+        <v>520</v>
+      </c>
+      <c r="C48" t="s">
         <v>185</v>
       </c>
-      <c r="D47" t="s">
-        <v>511</v>
-      </c>
-      <c r="E47" t="s">
-        <v>512</v>
-      </c>
-      <c r="F47" t="s">
-        <v>513</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="H47" t="s">
-        <v>515</v>
-      </c>
-      <c r="I47" t="s">
-        <v>515</v>
-      </c>
-      <c r="J47" s="3">
+      <c r="D48" t="s">
+        <v>521</v>
+      </c>
+      <c r="E48" t="s">
+        <v>522</v>
+      </c>
+      <c r="F48" t="s">
+        <v>523</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="H48" t="s">
+        <v>525</v>
+      </c>
+      <c r="I48" t="s">
+        <v>525</v>
+      </c>
+      <c r="J48" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80532_northumberland", ".\export_data\inspection_reports\80532_northumberland")</f>
         <v>0</v>
       </c>
-      <c r="K47" t="s">
-        <v>516</v>
-      </c>
-      <c r="L47" t="s">
-        <v>9</v>
-      </c>
-      <c r="M47" t="s">
-        <v>517</v>
-      </c>
-      <c r="N47" t="s">
-        <v>518</v>
-      </c>
-      <c r="O47" t="s">
-        <v>9</v>
-      </c>
-      <c r="P47" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q47" t="s">
+      <c r="K48" t="s">
+        <v>526</v>
+      </c>
+      <c r="L48" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" t="s">
+        <v>527</v>
+      </c>
+      <c r="N48" t="s">
+        <v>528</v>
+      </c>
+      <c r="O48" t="s">
+        <v>9</v>
+      </c>
+      <c r="P48" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q48" t="s">
         <v>82</v>
       </c>
-      <c r="R47" t="s">
-        <v>519</v>
+      <c r="R48" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -4722,6 +4809,7 @@
     <hyperlink ref="G45" r:id="rId44"/>
     <hyperlink ref="G46" r:id="rId45"/>
     <hyperlink ref="G47" r:id="rId46"/>
+    <hyperlink ref="G48" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>